<commit_message>
Update Real GDP Growth (IMF).xlsx
</commit_message>
<xml_diff>
--- a/Python Sessions/Real GDP Growth (IMF).xlsx
+++ b/Python Sessions/Real GDP Growth (IMF).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saeed Saffari\Documents\GitHub\alzahra-workshop-spr2021\lecture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saeed/Documents/GitHub/R_Python_workshop_ARDC_Win_2026/Python Sessions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BE2EF6-84C2-449B-997E-B41B8897876D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17156DA-E723-7E4C-B86A-D969BEAA6141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{77E7FE06-2D55-4C1D-BAF0-D09914AA89A1}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="38400" windowHeight="23400" activeTab="1" xr2:uid="{77E7FE06-2D55-4C1D-BAF0-D09914AA89A1}"/>
   </bookViews>
   <sheets>
     <sheet name="growth_1" sheetId="1" r:id="rId1"/>
@@ -912,9 +912,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -952,7 +952,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1058,7 +1058,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1200,7 +1200,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1210,24 +1210,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5161B4-8A43-4A5B-BCB9-A83149EE81B1}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="137" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="1"/>
+    <col min="6" max="6" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>1980</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1981</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1982</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1983</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>1984</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>1985</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>1986</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>1987</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>1988</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1989</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>1990</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>1991</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>1992</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>1993</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>1994</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>1995</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>1996</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>1997</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>1998</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>1999</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>2000</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>2001</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>2002</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>2003</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>2004</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>2005</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>2006</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>2007</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>2008</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>2009</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>2010</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>2011</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>2012</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>2013</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>2014</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>2015</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>2016</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>2017</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>2018</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>2019</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>2020</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>-3.5</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>2021</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>2022</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>2023</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>2024</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>2025</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>2026</v>
       </c>
@@ -2484,17 +2484,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E015F8A9-005F-4B74-91AA-EDC7784DCEC1}">
   <dimension ref="A1:B195"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="48.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>173</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>-3.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>175</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>-17.3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>176</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>-7.6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>-25.5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>-6.6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>-4.3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>-16.3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>-5.4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>-17.600000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>-6.4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>-14.1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>-7.7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>177</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>178</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>-8.3000000000000007</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>-4.0999999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>-3.8</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>179</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>-1.3</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>-3.5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>-2.8</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>2</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>-5.4</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>180</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>31</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>32</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>-5.8</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>174</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>33</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>-6.8</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>34</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>35</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>36</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>-7.8</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>37</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>-4.8</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>39</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>40</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>-5.0999999999999996</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>41</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>-5.6</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>38</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>42</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>-3.3</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>43</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>44</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>-10.4</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>45</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>-6.7</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>46</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>-7.5</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>47</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>48</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>-8.6</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>49</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>-5.8</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>50</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>51</v>
       </c>
@@ -2942,7 +2942,7 @@
         <v>-2.9</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>52</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>-3.3</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>53</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>54</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>-19</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>55</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>-2.9</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>56</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>-8.1999999999999993</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>57</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>58</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>59</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>-6.1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>60</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>-4.9000000000000004</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>181</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>61</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>-8.1999999999999993</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>182</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>-13.5</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>62</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>63</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>64</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>183</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>43.4</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>65</v>
       </c>
@@ -3078,7 +3078,7 @@
         <v>-3.7</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>66</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>67</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>-6.1</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>68</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>69</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>-6.6</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>70</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>71</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>-2.1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>3</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>72</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>-10.9</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>73</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>74</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>75</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>-8.9</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>76</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>-10.199999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>77</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>-4.8</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>78</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>79</v>
       </c>
@@ -3198,7 +3198,7 @@
         <v>-2.6</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>80</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>81</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>82</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>83</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>84</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>-8.1</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>85</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>86</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>87</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>-3.6</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>88</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>-25</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>89</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>-4.5</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>90</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>91</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>-59.7</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>92</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>93</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>-1.3</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>184</v>
       </c>
@@ -3318,7 +3318,7 @@
         <v>-56.3</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>94</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>-4.2</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>95</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>96</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>-5.6</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>97</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>-32.200000000000003</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>98</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>99</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>100</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>-3.3</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>101</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>-2.2000000000000002</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>102</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>-15.8</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>103</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>-8.1999999999999993</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>104</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>105</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>-7.5</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>106</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>-5.3</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>107</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>-15.2</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>108</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>109</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>110</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>185</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>-7.2</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>186</v>
       </c>
@@ -3470,7 +3470,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>111</v>
       </c>
@@ -3478,7 +3478,7 @@
         <v>-1.9</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>112</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>-3.8</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>113</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>114</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>115</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>116</v>
       </c>
@@ -3518,7 +3518,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>187</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>-4.5</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>4</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>117</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>-6.4</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>118</v>
       </c>
@@ -3550,7 +3550,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>119</v>
       </c>
@@ -3558,7 +3558,7 @@
         <v>-10.3</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>188</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>-17.899999999999999</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>120</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>-3.9</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>121</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>122</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>-11.1</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
         <v>123</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>-9.5</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>124</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>-2.7</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>125</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>-7.6</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>126</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>-7.5</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
         <v>127</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>-2.6</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
         <v>128</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>-3.9</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
         <v>129</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>-3.1</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
         <v>130</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
         <v>131</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>-18.7</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
         <v>132</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>-18.899999999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
         <v>189</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>-4.2</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
         <v>133</v>
       </c>
@@ -3686,7 +3686,7 @@
         <v>-3.2</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
         <v>134</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>-9.6999999999999993</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
         <v>136</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>-4.0999999999999996</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
         <v>137</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
         <v>138</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
         <v>139</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>-13.4</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
         <v>140</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>-2.2000000000000002</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
         <v>141</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>-5.4</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
         <v>142</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>-5.2</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
         <v>143</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>-5.5</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
         <v>144</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>-4.3</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
         <v>145</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
         <v>190</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
         <v>191</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>-6.6</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
         <v>146</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
         <v>147</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>-3.6</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
         <v>148</v>
       </c>
@@ -3814,7 +3814,7 @@
         <v>-3.6</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
         <v>192</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>-13.5</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
         <v>149</v>
       </c>
@@ -3830,7 +3830,7 @@
         <v>-2.8</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
         <v>150</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
         <v>135</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>-6.5</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
         <v>193</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
         <v>151</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
         <v>152</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
         <v>153</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>-6.1</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
         <v>154</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>-6.8</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
         <v>155</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
         <v>156</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
         <v>157</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>-7.8</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="s">
         <v>158</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>-8.8000000000000007</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
         <v>159</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
         <v>160</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
         <v>161</v>
       </c>
@@ -3942,7 +3942,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
         <v>162</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>-2.1</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="s">
         <v>163</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>-4.2</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
         <v>164</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>-5.9</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
         <v>165</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>-9.9</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
         <v>5</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>-3.5</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
         <v>166</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>-5.7</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="s">
         <v>167</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" s="3" t="s">
         <v>168</v>
       </c>
@@ -4006,7 +4006,7 @@
         <v>-9.1999999999999993</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
         <v>169</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" s="3" t="s">
         <v>194</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
         <v>195</v>
       </c>
@@ -4030,7 +4030,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
         <v>170</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
         <v>171</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>-3.5</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>172</v>
       </c>

</xml_diff>